<commit_message>
Added changes to local databases
</commit_message>
<xml_diff>
--- a/upload/dataset.xlsx
+++ b/upload/dataset.xlsx
@@ -5,22 +5,22 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Robin\Desktop\H4G\RainNet\upload\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Robin\Pictures\Ruebin\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA4B5CD7-300C-4C20-92D7-0EF6C6D84049}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{3B6D7E8A-8A22-4760-84CB-0E91A32E6AE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{441E1320-11F6-4571-8DB7-DEB2E4B4A190}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{6B152E1B-2705-4836-B2DC-3336B7868072}"/>
   </bookViews>
   <sheets>
-    <sheet name="dataset_idukki" sheetId="1" r:id="rId1"/>
+    <sheet name="dataset.xlsx" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="18">
   <si>
     <t>Block</t>
   </si>
@@ -31,10 +31,16 @@
     <t>Actual (mm)</t>
   </si>
   <si>
+    <t xml:space="preserve">Percentage of Deviation </t>
+  </si>
+  <si>
     <t>drainage capacity</t>
   </si>
   <si>
     <t>Devikulam</t>
+  </si>
+  <si>
+    <t>-</t>
   </si>
   <si>
     <t>high</t>
@@ -68,9 +74,6 @@
   </si>
   <si>
     <t>Kattappana</t>
-  </si>
-  <si>
-    <t>Deviation %</t>
   </si>
 </sst>
 </file>
@@ -932,67 +935,91 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6404DAAC-BDA8-4F37-A557-76B275C412CC}">
-  <dimension ref="A1:R10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1746469C-14D2-4195-B001-B6439C32B9A3}">
+  <dimension ref="A1:AA10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P3" sqref="P3"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="2" max="2" width="11.08984375" customWidth="1"/>
-    <col min="3" max="3" width="13.90625" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1">
+        <v>45292</v>
+      </c>
+      <c r="C1" s="1">
+        <v>45292</v>
+      </c>
+      <c r="D1" s="1">
+        <v>45323</v>
+      </c>
+      <c r="E1" s="1">
+        <v>45323</v>
+      </c>
+      <c r="F1" s="1">
+        <v>45352</v>
+      </c>
+      <c r="G1" s="1">
+        <v>45352</v>
+      </c>
+      <c r="H1" s="1">
+        <v>45383</v>
+      </c>
+      <c r="I1" s="1">
+        <v>45383</v>
+      </c>
+      <c r="J1" s="1">
+        <v>45413</v>
+      </c>
+      <c r="K1" s="1">
+        <v>45413</v>
+      </c>
+      <c r="L1" s="1">
         <v>45444</v>
       </c>
-      <c r="C1" s="1">
+      <c r="M1" s="1">
         <v>45444</v>
       </c>
-      <c r="D1" s="1">
+      <c r="N1" s="1">
         <v>45474</v>
       </c>
-      <c r="E1" s="1">
+      <c r="O1" s="1">
         <v>45474</v>
       </c>
-      <c r="F1" s="1">
+      <c r="P1" s="1">
         <v>45505</v>
       </c>
-      <c r="G1" s="1">
+      <c r="Q1" s="1">
         <v>45505</v>
       </c>
-      <c r="H1" s="1">
+      <c r="R1" s="1">
         <v>45536</v>
       </c>
-      <c r="I1" s="1">
+      <c r="S1" s="1">
         <v>45536</v>
       </c>
-      <c r="J1" s="1">
+      <c r="T1" s="1">
         <v>45566</v>
       </c>
-      <c r="K1" s="1">
+      <c r="U1" s="1">
         <v>45566</v>
       </c>
-      <c r="L1" s="1">
+      <c r="V1" s="1">
         <v>45597</v>
       </c>
-      <c r="M1" s="1">
+      <c r="W1" s="1">
         <v>45597</v>
       </c>
-      <c r="N1" s="1">
+      <c r="X1" s="1">
         <v>45627</v>
       </c>
-      <c r="O1" s="1">
+      <c r="Y1" s="1">
         <v>45627</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
         <v>1</v>
       </c>
@@ -1036,434 +1063,704 @@
         <v>2</v>
       </c>
       <c r="P2" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>2</v>
+      </c>
+      <c r="R2" t="s">
+        <v>1</v>
+      </c>
+      <c r="S2" t="s">
+        <v>2</v>
+      </c>
+      <c r="T2" t="s">
+        <v>1</v>
+      </c>
+      <c r="U2" t="s">
+        <v>2</v>
+      </c>
+      <c r="V2" t="s">
+        <v>1</v>
+      </c>
+      <c r="W2" t="s">
+        <v>2</v>
+      </c>
+      <c r="X2" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>2</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>3</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3">
+        <v>19.7</v>
+      </c>
+      <c r="C3">
+        <v>76.599999999999994</v>
+      </c>
+      <c r="D3">
+        <v>12.9</v>
+      </c>
+      <c r="E3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3">
+        <v>93.1</v>
+      </c>
+      <c r="G3">
+        <v>14.8</v>
+      </c>
+      <c r="H3">
+        <v>202.8</v>
+      </c>
+      <c r="I3">
+        <v>13.9</v>
+      </c>
+      <c r="J3">
+        <v>193.7</v>
+      </c>
+      <c r="K3">
+        <v>349.7</v>
+      </c>
+      <c r="L3">
+        <v>225.3</v>
+      </c>
+      <c r="M3">
+        <v>371.5</v>
+      </c>
+      <c r="N3">
+        <v>584.1</v>
+      </c>
+      <c r="O3">
+        <v>608.1</v>
+      </c>
+      <c r="P3">
+        <v>185.4</v>
+      </c>
+      <c r="Q3">
+        <v>307.89999999999998</v>
+      </c>
+      <c r="R3">
+        <v>349.7</v>
+      </c>
+      <c r="S3">
+        <v>185.2</v>
+      </c>
+      <c r="T3">
+        <v>322.89999999999998</v>
+      </c>
+      <c r="U3">
+        <v>274.8</v>
+      </c>
+      <c r="V3">
+        <v>276.10000000000002</v>
+      </c>
+      <c r="W3">
+        <v>130.9</v>
+      </c>
+      <c r="X3">
+        <v>116</v>
+      </c>
+      <c r="Y3">
+        <v>151.30000000000001</v>
+      </c>
+      <c r="Z3" s="2">
+        <v>-3.7999999999999999E-2</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4">
+        <v>13.7</v>
+      </c>
+      <c r="C4">
+        <v>90.4</v>
+      </c>
+      <c r="D4">
+        <v>3.2</v>
+      </c>
+      <c r="E4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4">
+        <v>85.4</v>
+      </c>
+      <c r="G4">
+        <v>15.7</v>
+      </c>
+      <c r="H4">
+        <v>149.1</v>
+      </c>
+      <c r="I4">
+        <v>29.9</v>
+      </c>
+      <c r="J4">
+        <v>263.5</v>
+      </c>
+      <c r="K4">
+        <v>751</v>
+      </c>
+      <c r="L4">
+        <v>362.5</v>
+      </c>
+      <c r="M4">
+        <v>640.29999999999995</v>
+      </c>
+      <c r="N4">
+        <v>821.6</v>
+      </c>
+      <c r="O4">
+        <v>764.5</v>
+      </c>
+      <c r="P4">
+        <v>117.1</v>
+      </c>
+      <c r="Q4">
+        <v>492.1</v>
+      </c>
+      <c r="R4">
+        <v>457.1</v>
+      </c>
+      <c r="S4">
+        <v>281.7</v>
+      </c>
+      <c r="T4">
+        <v>406.5</v>
+      </c>
+      <c r="U4">
+        <v>386.3</v>
+      </c>
+      <c r="V4">
+        <v>249</v>
+      </c>
+      <c r="W4">
+        <v>201.2</v>
+      </c>
+      <c r="X4">
+        <v>77.400000000000006</v>
+      </c>
+      <c r="Y4">
+        <v>224.9</v>
+      </c>
+      <c r="Z4" s="2">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="AA4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5">
+        <v>23.3</v>
+      </c>
+      <c r="C5">
+        <v>86.7</v>
+      </c>
+      <c r="D5">
+        <v>6.9</v>
+      </c>
+      <c r="E5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F5">
+        <v>85.7</v>
+      </c>
+      <c r="G5">
+        <v>16.100000000000001</v>
+      </c>
+      <c r="H5">
+        <v>138.19999999999999</v>
+      </c>
+      <c r="I5">
+        <v>20.2</v>
+      </c>
+      <c r="J5">
+        <v>204.1</v>
+      </c>
+      <c r="K5">
+        <v>513.9</v>
+      </c>
+      <c r="L5">
+        <v>209.2</v>
+      </c>
+      <c r="M5">
+        <v>581.4</v>
+      </c>
+      <c r="N5">
+        <v>713.5</v>
+      </c>
+      <c r="O5">
+        <v>878</v>
+      </c>
+      <c r="P5">
+        <v>132.19999999999999</v>
+      </c>
+      <c r="Q5">
+        <v>471.8</v>
+      </c>
+      <c r="R5">
+        <v>302.89999999999998</v>
+      </c>
+      <c r="S5">
+        <v>296.10000000000002</v>
+      </c>
+      <c r="T5">
+        <v>284.2</v>
+      </c>
+      <c r="U5">
+        <v>406.3</v>
+      </c>
+      <c r="V5">
+        <v>230.8</v>
+      </c>
+      <c r="W5">
+        <v>155.1</v>
+      </c>
+      <c r="X5">
+        <v>92</v>
+      </c>
+      <c r="Y5">
+        <v>204.9</v>
+      </c>
+      <c r="Z5" s="2">
+        <v>0.498</v>
+      </c>
+      <c r="AA5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6">
+        <v>11.6</v>
+      </c>
+      <c r="C6">
+        <v>53.5</v>
+      </c>
+      <c r="D6">
+        <v>5.4</v>
+      </c>
+      <c r="E6">
+        <v>0.3</v>
+      </c>
+      <c r="F6">
+        <v>63.9</v>
+      </c>
+      <c r="G6">
+        <v>32.299999999999997</v>
+      </c>
+      <c r="H6">
+        <v>111.8</v>
+      </c>
+      <c r="I6">
+        <v>19.399999999999999</v>
+      </c>
+      <c r="J6">
+        <v>119.9</v>
+      </c>
+      <c r="K6">
+        <v>438.6</v>
+      </c>
+      <c r="L6">
+        <v>58.5</v>
+      </c>
+      <c r="M6">
+        <v>489.4</v>
+      </c>
+      <c r="N6">
+        <v>211.7</v>
+      </c>
+      <c r="O6">
+        <v>607.1</v>
+      </c>
+      <c r="P6">
+        <v>36.6</v>
+      </c>
+      <c r="Q6">
+        <v>355.5</v>
+      </c>
+      <c r="R6">
+        <v>122.1</v>
+      </c>
+      <c r="S6">
+        <v>181</v>
+      </c>
+      <c r="T6">
+        <v>249.8</v>
+      </c>
+      <c r="U6">
+        <v>252.6</v>
+      </c>
+      <c r="V6">
+        <v>367.5</v>
+      </c>
+      <c r="W6">
+        <v>140</v>
+      </c>
+      <c r="X6">
+        <v>164.1</v>
+      </c>
+      <c r="Y6">
+        <v>247.4</v>
+      </c>
+      <c r="Z6" s="2">
+        <v>0.85</v>
+      </c>
+      <c r="AA6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7">
+        <v>17.899999999999999</v>
+      </c>
+      <c r="C7">
+        <v>83.7</v>
+      </c>
+      <c r="D7">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="E7" t="s">
+        <v>6</v>
+      </c>
+      <c r="F7">
+        <v>83.5</v>
+      </c>
+      <c r="G7">
+        <v>15.6</v>
+      </c>
+      <c r="H7">
+        <v>140.69999999999999</v>
+      </c>
+      <c r="I7">
+        <v>22.3</v>
+      </c>
+      <c r="J7">
+        <v>238.8</v>
+      </c>
+      <c r="K7">
+        <v>634.1</v>
+      </c>
+      <c r="L7">
+        <v>286.10000000000002</v>
+      </c>
+      <c r="M7">
+        <v>699</v>
+      </c>
+      <c r="N7">
+        <v>758.2</v>
+      </c>
+      <c r="O7">
+        <v>962.9</v>
+      </c>
+      <c r="P7">
+        <v>115.9</v>
+      </c>
+      <c r="Q7">
+        <v>545.6</v>
+      </c>
+      <c r="R7">
+        <v>378.6</v>
+      </c>
+      <c r="S7">
+        <v>326.8</v>
+      </c>
+      <c r="T7">
+        <v>354</v>
+      </c>
+      <c r="U7">
+        <v>450.6</v>
+      </c>
+      <c r="V7">
+        <v>247.5</v>
+      </c>
+      <c r="W7">
+        <v>171.4</v>
+      </c>
+      <c r="X7">
+        <v>83.1</v>
+      </c>
+      <c r="Y7">
+        <v>219.8</v>
+      </c>
+      <c r="Z7" s="2">
+        <v>0.52500000000000002</v>
+      </c>
+      <c r="AA7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8">
+        <v>14.2</v>
+      </c>
+      <c r="C8">
+        <v>77.900000000000006</v>
+      </c>
+      <c r="D8">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="E8" t="s">
+        <v>6</v>
+      </c>
+      <c r="F8">
+        <v>58</v>
+      </c>
+      <c r="G8">
+        <v>15.4</v>
+      </c>
+      <c r="H8">
+        <v>107.5</v>
+      </c>
+      <c r="I8">
+        <v>16.600000000000001</v>
+      </c>
+      <c r="J8">
+        <v>185.7</v>
+      </c>
+      <c r="K8">
+        <v>557</v>
+      </c>
+      <c r="L8">
+        <v>131.9</v>
+      </c>
+      <c r="M8">
+        <v>628</v>
+      </c>
+      <c r="N8">
+        <v>480.5</v>
+      </c>
+      <c r="O8">
+        <v>882.5</v>
+      </c>
+      <c r="P8">
+        <v>67.8</v>
+      </c>
+      <c r="Q8">
+        <v>428.8</v>
+      </c>
+      <c r="R8" t="s">
+        <v>15</v>
+      </c>
+      <c r="S8">
+        <v>268.39999999999998</v>
+      </c>
+      <c r="T8">
+        <v>339.7</v>
+      </c>
+      <c r="U8">
+        <v>334.3</v>
+      </c>
+      <c r="V8">
+        <v>312.3</v>
+      </c>
+      <c r="W8">
+        <v>138.5</v>
+      </c>
+      <c r="X8">
+        <v>121</v>
+      </c>
+      <c r="Y8">
+        <v>218.5</v>
+      </c>
+      <c r="Z8" s="2">
+        <v>0.74299999999999999</v>
+      </c>
+      <c r="AA8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
         <v>16</v>
       </c>
-      <c r="R2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3">
-        <v>225.3</v>
-      </c>
-      <c r="C3">
-        <v>371.5</v>
-      </c>
-      <c r="D3">
-        <v>584.1</v>
-      </c>
-      <c r="E3">
-        <v>608.1</v>
-      </c>
-      <c r="F3">
-        <v>185.4</v>
-      </c>
-      <c r="G3">
-        <v>307.89999999999998</v>
-      </c>
-      <c r="H3">
-        <v>349.7</v>
-      </c>
-      <c r="I3">
-        <v>185.2</v>
-      </c>
-      <c r="J3">
-        <v>322.89999999999998</v>
-      </c>
-      <c r="K3">
-        <v>274.8</v>
-      </c>
-      <c r="L3">
-        <v>276.10000000000002</v>
-      </c>
-      <c r="M3">
-        <v>130.9</v>
-      </c>
-      <c r="N3">
-        <v>116</v>
-      </c>
-      <c r="O3">
-        <v>151.30000000000001</v>
-      </c>
-      <c r="P3" s="2">
-        <v>9.5000000000000001E-2</v>
-      </c>
-      <c r="R3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
+      <c r="B9">
+        <v>8.4</v>
+      </c>
+      <c r="C9">
+        <v>80.2</v>
+      </c>
+      <c r="D9">
+        <v>9.6999999999999993</v>
+      </c>
+      <c r="E9" t="s">
         <v>6</v>
       </c>
-      <c r="B4">
-        <v>362.5</v>
-      </c>
-      <c r="C4">
-        <v>640.29999999999995</v>
-      </c>
-      <c r="D4">
-        <v>821.6</v>
-      </c>
-      <c r="E4">
-        <v>764.5</v>
-      </c>
-      <c r="F4">
-        <v>117.1</v>
-      </c>
-      <c r="G4">
-        <v>492.1</v>
-      </c>
-      <c r="H4">
-        <v>457.1</v>
-      </c>
-      <c r="I4">
-        <v>281.7</v>
-      </c>
-      <c r="J4">
-        <v>406.5</v>
-      </c>
-      <c r="K4">
-        <v>386.3</v>
-      </c>
-      <c r="L4">
-        <v>249</v>
-      </c>
-      <c r="M4">
-        <v>201.2</v>
-      </c>
-      <c r="N4">
-        <v>77.400000000000006</v>
-      </c>
-      <c r="O4">
-        <v>224.9</v>
-      </c>
-      <c r="P4" s="2">
-        <v>0.23899999999999999</v>
-      </c>
-      <c r="R4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5">
-        <v>209.2</v>
-      </c>
-      <c r="C5">
-        <v>581.4</v>
-      </c>
-      <c r="D5">
-        <v>713.5</v>
-      </c>
-      <c r="E5">
-        <v>878</v>
-      </c>
-      <c r="F5">
-        <v>132.19999999999999</v>
-      </c>
-      <c r="G5">
-        <v>471.8</v>
-      </c>
-      <c r="H5">
-        <v>302.89999999999998</v>
-      </c>
-      <c r="I5">
-        <v>296.10000000000002</v>
-      </c>
-      <c r="J5">
-        <v>284.2</v>
-      </c>
-      <c r="K5">
-        <v>406.3</v>
-      </c>
-      <c r="L5">
-        <v>230.8</v>
-      </c>
-      <c r="M5">
-        <v>155.1</v>
-      </c>
-      <c r="N5">
-        <v>92</v>
-      </c>
-      <c r="O5">
-        <v>204.9</v>
-      </c>
-      <c r="P5" s="2">
-        <v>0.64</v>
-      </c>
-      <c r="R5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6">
-        <v>58.5</v>
-      </c>
-      <c r="C6">
-        <v>489.4</v>
-      </c>
-      <c r="D6">
-        <v>211.7</v>
-      </c>
-      <c r="E6">
-        <v>607.1</v>
-      </c>
-      <c r="F6">
-        <v>36.6</v>
-      </c>
-      <c r="G6">
-        <v>355.5</v>
-      </c>
-      <c r="H6">
-        <v>122.1</v>
-      </c>
-      <c r="I6">
-        <v>181</v>
-      </c>
-      <c r="J6">
-        <v>249.8</v>
-      </c>
-      <c r="K6">
-        <v>252.6</v>
-      </c>
-      <c r="L6">
-        <v>367.5</v>
-      </c>
-      <c r="M6">
-        <v>140</v>
-      </c>
-      <c r="N6">
-        <v>164.1</v>
-      </c>
-      <c r="O6">
-        <v>247.4</v>
-      </c>
-      <c r="P6" s="2">
-        <v>2.8069999999999999</v>
-      </c>
-      <c r="R6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7">
-        <v>286.10000000000002</v>
-      </c>
-      <c r="C7">
-        <v>699</v>
-      </c>
-      <c r="D7">
-        <v>758.2</v>
-      </c>
-      <c r="E7">
-        <v>962.9</v>
-      </c>
-      <c r="F7">
-        <v>115.9</v>
-      </c>
-      <c r="G7">
-        <v>545.6</v>
-      </c>
-      <c r="H7">
-        <v>378.6</v>
-      </c>
-      <c r="I7">
-        <v>326.8</v>
-      </c>
-      <c r="J7">
-        <v>354</v>
-      </c>
-      <c r="K7">
-        <v>450.6</v>
-      </c>
-      <c r="L7">
-        <v>247.5</v>
-      </c>
-      <c r="M7">
-        <v>171.4</v>
-      </c>
-      <c r="N7">
-        <v>83.1</v>
-      </c>
-      <c r="O7">
-        <v>219.8</v>
-      </c>
-      <c r="P7" s="2">
-        <v>0.64700000000000002</v>
-      </c>
-      <c r="R7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8">
-        <v>131.9</v>
-      </c>
-      <c r="C8">
-        <v>628</v>
-      </c>
-      <c r="D8">
-        <v>480.5</v>
-      </c>
-      <c r="E8">
-        <v>882.5</v>
-      </c>
-      <c r="F8">
-        <v>67.8</v>
-      </c>
-      <c r="G8">
-        <v>428.8</v>
-      </c>
-      <c r="H8" t="s">
-        <v>13</v>
-      </c>
-      <c r="I8">
-        <v>268.39999999999998</v>
-      </c>
-      <c r="J8">
-        <v>339.7</v>
-      </c>
-      <c r="K8">
-        <v>334.3</v>
-      </c>
-      <c r="L8">
-        <v>312.3</v>
-      </c>
-      <c r="M8">
-        <v>138.5</v>
-      </c>
-      <c r="N8">
-        <v>121</v>
-      </c>
-      <c r="O8">
-        <v>218.5</v>
-      </c>
-      <c r="P8" s="2">
-        <v>1.4550000000000001</v>
-      </c>
-      <c r="R8" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>14</v>
-      </c>
-      <c r="B9">
-        <v>131.9</v>
-      </c>
-      <c r="C9">
-        <v>628</v>
-      </c>
-      <c r="D9">
-        <v>161</v>
-      </c>
-      <c r="E9">
-        <v>640.70000000000005</v>
-      </c>
       <c r="F9">
-        <v>44.1</v>
+        <v>24.4</v>
       </c>
       <c r="G9">
-        <v>243.4</v>
+        <v>17</v>
       </c>
       <c r="H9">
         <v>79.3</v>
       </c>
       <c r="I9">
+        <v>12.3</v>
+      </c>
+      <c r="J9">
+        <v>104.8</v>
+      </c>
+      <c r="K9">
+        <v>330.2</v>
+      </c>
+      <c r="L9">
+        <v>131.9</v>
+      </c>
+      <c r="M9">
+        <v>628</v>
+      </c>
+      <c r="N9">
+        <v>161</v>
+      </c>
+      <c r="O9">
+        <v>640.70000000000005</v>
+      </c>
+      <c r="P9">
+        <v>44.1</v>
+      </c>
+      <c r="Q9">
+        <v>243.4</v>
+      </c>
+      <c r="R9">
+        <v>79.3</v>
+      </c>
+      <c r="S9">
         <v>172.4</v>
       </c>
-      <c r="J9">
+      <c r="T9">
         <v>154.5</v>
       </c>
-      <c r="K9">
+      <c r="U9">
         <v>253.1</v>
       </c>
-      <c r="L9">
+      <c r="V9">
         <v>288</v>
       </c>
-      <c r="M9">
+      <c r="W9">
         <v>108.7</v>
       </c>
-      <c r="N9">
+      <c r="X9">
         <v>101.8</v>
       </c>
-      <c r="O9">
+      <c r="Y9">
         <v>194.2</v>
       </c>
-      <c r="P9" s="2">
-        <v>3.339</v>
-      </c>
-      <c r="R9" t="s">
-        <v>10</v>
+      <c r="Z9" s="2">
+        <v>1.2110000000000001</v>
+      </c>
+      <c r="AA9" t="s">
+        <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B10">
+        <v>11.1</v>
+      </c>
+      <c r="C10">
+        <v>73</v>
+      </c>
+      <c r="D10">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="E10" t="s">
+        <v>6</v>
+      </c>
+      <c r="F10">
+        <v>37.799999999999997</v>
+      </c>
+      <c r="G10">
+        <v>25.3</v>
+      </c>
+      <c r="H10">
+        <v>82.7</v>
+      </c>
+      <c r="I10">
+        <v>11.5</v>
+      </c>
+      <c r="J10">
+        <v>145.80000000000001</v>
+      </c>
+      <c r="K10">
+        <v>367</v>
+      </c>
+      <c r="L10">
         <v>56.5</v>
       </c>
-      <c r="C10">
+      <c r="M10">
         <v>453.8</v>
       </c>
-      <c r="D10">
+      <c r="N10">
         <v>280.3</v>
       </c>
-      <c r="E10">
+      <c r="O10">
         <v>652.9</v>
       </c>
-      <c r="F10">
+      <c r="P10">
         <v>35.700000000000003</v>
       </c>
-      <c r="G10">
+      <c r="Q10">
         <v>273.3</v>
       </c>
-      <c r="H10">
+      <c r="R10">
         <v>124.3</v>
       </c>
-      <c r="I10">
+      <c r="S10">
         <v>168.7</v>
       </c>
-      <c r="J10">
+      <c r="T10">
         <v>270.39999999999998</v>
       </c>
-      <c r="K10">
+      <c r="U10">
         <v>233.4</v>
       </c>
-      <c r="L10">
+      <c r="V10">
         <v>326.7</v>
       </c>
-      <c r="M10">
+      <c r="W10">
         <v>106.7</v>
       </c>
-      <c r="N10">
+      <c r="X10">
         <v>118</v>
       </c>
-      <c r="O10">
+      <c r="Y10">
         <v>227.4</v>
       </c>
-      <c r="P10" s="2">
-        <v>2.117</v>
-      </c>
-      <c r="R10" t="s">
-        <v>10</v>
+      <c r="Z10" s="2">
+        <v>0.73099999999999998</v>
+      </c>
+      <c r="AA10" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>